<commit_message>
Provider Dupe Logic Added
Duplicate Providers can cause issues, SO we added simple logic to check
for such issues.
</commit_message>
<xml_diff>
--- a/working/providers/Providers_Dummy.xlsx
+++ b/working/providers/Providers_Dummy.xlsx
@@ -40,6 +40,21 @@
     <t>david.larrimore@gmail.com</t>
   </si>
   <si>
+    <t>xlsx</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>MRO</t>
+  </si>
+  <si>
+    <t>GS23FBA017</t>
+  </si>
+  <si>
+    <t>david.larrimore@gmail.com</t>
+  </si>
+  <si>
     <t>csv</t>
   </si>
   <si>
@@ -49,7 +64,7 @@
     <t>MRO</t>
   </si>
   <si>
-    <t>GS23FBA017</t>
+    <t>GS23FBA011</t>
   </si>
   <si>
     <t>david.larrimore@gmail.com</t>
@@ -178,6 +193,23 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4">
+      <c t="s" s="2" r="A4">
+        <v>15</v>
+      </c>
+      <c t="s" s="2" r="B4">
+        <v>16</v>
+      </c>
+      <c t="s" s="2" r="C4">
+        <v>17</v>
+      </c>
+      <c t="s" s="2" r="D4">
+        <v>18</v>
+      </c>
+      <c t="s" s="2" r="E4">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>